<commit_message>
Improved table and listings, saved some widows and orphans.
</commit_message>
<xml_diff>
--- a/paper-aplas/known_issues_readable.xlsx
+++ b/paper-aplas/known_issues_readable.xlsx
@@ -293,7 +293,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -301,6 +301,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -317,7 +322,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,13 +337,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="15"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -354,8 +353,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -367,14 +378,73 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -382,12 +452,53 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color indexed="10"/>
-      </top>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="10"/>
       </bottom>
@@ -399,56 +510,83 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,24 +597,24 @@
     <dxf>
       <font>
         <b val="1"/>
-        <color rgb="00000000"/>
+        <color rgb="ff000000"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="12"/>
-          <bgColor indexed="13"/>
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
         <b val="1"/>
-        <color rgb="00000000"/>
+        <color rgb="ff000000"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <fgColor indexed="12"/>
-          <bgColor indexed="13"/>
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
         </patternFill>
       </fill>
     </dxf>
@@ -493,8 +631,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="fffe634d"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="00000000"/>
       <rgbColor rgb="ff919191"/>
@@ -518,10 +658,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -698,11 +838,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -711,27 +854,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -988,10 +1131,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1282,7 +1425,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1563,366 +1706,514 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:B49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B1" xSplit="1" ySplit="0" activePane="topRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="57.1094" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.8828" style="1" customWidth="1"/>
-    <col min="3" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="57.1719" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.8516" style="1" customWidth="1"/>
+    <col min="3" max="5" width="16.3516" style="1" customWidth="1"/>
+    <col min="6" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" ht="44.05" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="6">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="7">
         <v>2</v>
       </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="5">
+      <c r="A3" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="6">
+      <c r="B3" t="s" s="12">
         <v>4</v>
       </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="7">
+      <c r="A4" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="6">
+      <c r="B4" t="s" s="12">
         <v>6</v>
       </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
-      <c r="A5" t="s" s="8">
+      <c r="A5" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" t="s" s="10">
+      <c r="A6" t="s" s="16">
         <v>8</v>
       </c>
-      <c r="B6" t="s" s="4">
+      <c r="B6" t="s" s="7">
         <v>9</v>
       </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="32.05" customHeight="1">
-      <c r="A7" t="s" s="11">
+      <c r="A7" t="s" s="17">
         <v>10</v>
       </c>
-      <c r="B7" t="s" s="4">
+      <c r="B7" t="s" s="7">
         <v>11</v>
       </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="32.05" customHeight="1">
-      <c r="A8" t="s" s="7">
+      <c r="A8" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="B8" t="s" s="4">
+      <c r="B8" t="s" s="7">
         <v>13</v>
       </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="32.05" customHeight="1">
-      <c r="A9" t="s" s="7">
+      <c r="A9" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="B9" t="s" s="6">
+      <c r="B9" t="s" s="12">
         <v>15</v>
       </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="8">
+      <c r="A10" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="B10" t="s" s="4">
+      <c r="B10" t="s" s="7">
         <v>17</v>
       </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" ht="32.05" customHeight="1">
-      <c r="A11" t="s" s="5">
+      <c r="A11" t="s" s="11">
         <v>18</v>
       </c>
-      <c r="B11" t="s" s="4">
+      <c r="B11" t="s" s="7">
         <v>19</v>
       </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" ht="68.05" customHeight="1">
-      <c r="A12" t="s" s="10">
+      <c r="A12" t="s" s="16">
         <v>20</v>
       </c>
-      <c r="B12" t="s" s="12">
+      <c r="B12" t="s" s="18">
         <v>21</v>
       </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="7">
+      <c r="A13" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="B13" t="s" s="6">
+      <c r="B13" t="s" s="12">
         <v>15</v>
       </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" ht="32.05" customHeight="1">
-      <c r="A14" t="s" s="13">
+      <c r="A14" t="s" s="19">
         <v>23</v>
       </c>
-      <c r="B14" t="s" s="6">
+      <c r="B14" t="s" s="12">
         <v>15</v>
       </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" ht="32.05" customHeight="1">
-      <c r="A15" t="s" s="8">
+      <c r="A15" t="s" s="14">
         <v>24</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" ht="32.05" customHeight="1">
-      <c r="A16" t="s" s="13">
+      <c r="A16" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="B16" t="s" s="6">
+      <c r="B16" t="s" s="12">
         <v>15</v>
       </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" ht="44.05" customHeight="1">
-      <c r="A17" t="s" s="8">
+      <c r="A17" t="s" s="14">
         <v>26</v>
       </c>
-      <c r="B17" t="s" s="4">
+      <c r="B17" t="s" s="7">
         <v>27</v>
       </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" ht="56.05" customHeight="1">
-      <c r="A18" t="s" s="8">
+      <c r="A18" t="s" s="14">
         <v>28</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" ht="32.05" customHeight="1">
-      <c r="A19" t="s" s="7">
+      <c r="A19" t="s" s="13">
         <v>29</v>
       </c>
-      <c r="B19" t="s" s="6">
+      <c r="B19" t="s" s="12">
         <v>15</v>
       </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" ht="44.05" customHeight="1">
-      <c r="A20" t="s" s="13">
+      <c r="A20" t="s" s="19">
         <v>30</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" ht="56.05" customHeight="1">
-      <c r="A21" t="s" s="13">
+      <c r="A21" t="s" s="19">
         <v>31</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="13">
+      <c r="A22" t="s" s="19">
         <v>32</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" ht="32.05" customHeight="1">
-      <c r="A23" t="s" s="7">
+      <c r="A23" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="B23" t="s" s="6">
+      <c r="B23" t="s" s="12">
         <v>15</v>
       </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="13">
+      <c r="A24" t="s" s="19">
         <v>34</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" t="s" s="7">
+        <v>15</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" ht="48" customHeight="1">
-      <c r="A25" t="s" s="13">
+      <c r="A25" t="s" s="19">
         <v>35</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="13">
+      <c r="A26" t="s" s="19">
         <v>36</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="14"/>
-      <c r="B27" s="9"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="14"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" ht="32.05" customHeight="1">
-      <c r="A29" t="s" s="13">
+      <c r="A29" t="s" s="19">
         <v>37</v>
       </c>
-      <c r="B29" t="s" s="4">
+      <c r="B29" t="s" s="7">
         <v>38</v>
       </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" ht="44.05" customHeight="1">
-      <c r="A30" t="s" s="13">
+      <c r="A30" t="s" s="19">
         <v>39</v>
       </c>
-      <c r="B30" t="s" s="4">
+      <c r="B30" t="s" s="7">
         <v>40</v>
       </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" ht="44.05" customHeight="1">
-      <c r="A31" t="s" s="15">
+      <c r="A31" t="s" s="21">
         <v>41</v>
       </c>
-      <c r="B31" t="s" s="4">
+      <c r="B31" t="s" s="7">
         <v>42</v>
       </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" ht="44.05" customHeight="1">
-      <c r="A32" t="s" s="15">
+      <c r="A32" t="s" s="21">
         <v>43</v>
       </c>
-      <c r="B32" t="s" s="4">
+      <c r="B32" t="s" s="7">
         <v>15</v>
       </c>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" ht="32.05" customHeight="1">
-      <c r="A33" t="s" s="13">
+      <c r="A33" t="s" s="19">
         <v>44</v>
       </c>
-      <c r="B33" t="s" s="4">
+      <c r="B33" t="s" s="7">
         <v>45</v>
       </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" ht="44.05" customHeight="1">
-      <c r="A34" t="s" s="13">
+      <c r="A34" t="s" s="19">
         <v>46</v>
       </c>
-      <c r="B34" t="s" s="4">
+      <c r="B34" t="s" s="7">
         <v>47</v>
       </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" ht="61.45" customHeight="1">
-      <c r="A35" t="s" s="13">
+      <c r="A35" t="s" s="19">
         <v>48</v>
       </c>
-      <c r="B35" t="s" s="4">
+      <c r="B35" t="s" s="7">
         <v>15</v>
       </c>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" ht="32.05" customHeight="1">
-      <c r="A36" t="s" s="15">
+      <c r="A36" t="s" s="21">
         <v>49</v>
       </c>
-      <c r="B36" t="s" s="4">
+      <c r="B36" t="s" s="7">
         <v>50</v>
       </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" ht="68.05" customHeight="1">
-      <c r="A37" t="s" s="13">
+      <c r="A37" t="s" s="19">
         <v>51</v>
       </c>
-      <c r="B37" t="s" s="4">
+      <c r="B37" t="s" s="7">
         <v>52</v>
       </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" ht="56.05" customHeight="1">
-      <c r="A38" t="s" s="15">
+      <c r="A38" t="s" s="21">
         <v>53</v>
       </c>
-      <c r="B38" t="s" s="4">
+      <c r="B38" t="s" s="7">
         <v>54</v>
       </c>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" ht="68.05" customHeight="1">
-      <c r="A39" t="s" s="15">
+      <c r="A39" t="s" s="21">
         <v>55</v>
       </c>
-      <c r="B39" t="s" s="4">
+      <c r="B39" t="s" s="7">
         <v>50</v>
       </c>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" ht="32.05" customHeight="1">
-      <c r="A40" t="s" s="13">
+      <c r="A40" t="s" s="19">
         <v>56</v>
       </c>
-      <c r="B40" t="s" s="4">
+      <c r="B40" t="s" s="7">
         <v>50</v>
       </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" ht="32.05" customHeight="1">
-      <c r="A41" t="s" s="16">
+      <c r="A41" t="s" s="22">
         <v>57</v>
       </c>
-      <c r="B41" s="9"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" ht="32.05" customHeight="1">
-      <c r="A42" t="s" s="16">
+      <c r="A42" t="s" s="22">
         <v>58</v>
       </c>
-      <c r="B42" s="9"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" ht="32.05" customHeight="1">
-      <c r="A43" t="s" s="16">
+      <c r="A43" t="s" s="22">
         <v>59</v>
       </c>
-      <c r="B43" s="9"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" ht="92.05" customHeight="1">
-      <c r="A44" t="s" s="16">
+      <c r="A44" t="s" s="22">
         <v>60</v>
       </c>
-      <c r="B44" s="9"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" ht="44.05" customHeight="1">
-      <c r="A45" t="s" s="15">
+      <c r="A45" t="s" s="21">
         <v>61</v>
       </c>
-      <c r="B45" t="s" s="4">
+      <c r="B45" t="s" s="7">
         <v>62</v>
       </c>
+      <c r="C45" s="8"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="32.05" customHeight="1">
-      <c r="A46" t="s" s="16">
+      <c r="A46" t="s" s="22">
         <v>63</v>
       </c>
-      <c r="B46" s="9"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" ht="44.05" customHeight="1">
-      <c r="A47" t="s" s="16">
+      <c r="A47" t="s" s="22">
         <v>64</v>
       </c>
-      <c r="B47" s="9"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" ht="44.05" customHeight="1">
-      <c r="A48" t="s" s="16">
+      <c r="A48" t="s" s="22">
         <v>65</v>
       </c>
-      <c r="B48" s="9"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" ht="44.05" customHeight="1">
-      <c r="A49" t="s" s="16">
+      <c r="A49" t="s" s="22">
         <v>66</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Handled issue 6, tightened related work, added bib ref.
</commit_message>
<xml_diff>
--- a/paper-aplas/known_issues_readable.xlsx
+++ b/paper-aplas/known_issues_readable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
   <si>
     <t>Table 1</t>
   </si>
@@ -47,7 +47,7 @@
     <t>6. Acknowledge Charguéraud and Pottier's repeater when introducing repeater</t>
   </si>
   <si>
-    <t>Anshuman.</t>
+    <t>Done.</t>
   </si>
   <si>
     <t>7. Add a disclaimer that the practical hardcoded solution is obvious, we are trying to win in theory-land</t>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">8. I think A(m, n) should have a different notation than the diagonal A(n). </t>
-  </si>
-  <si>
-    <t>Done.</t>
   </si>
   <si>
     <t>9. Shall we remove the pedantic sub_2 from Section 5.2?</t>
@@ -196,6 +193,12 @@
   </si>
   <si>
     <t>Th 41. \forall i</t>
+  </si>
+  <si>
+    <t>Re-link to new repo</t>
+  </si>
+  <si>
+    <t>Anshuman changed some function names to make the listings fit, please reflect in codebase and in writing.</t>
   </si>
   <si>
     <t>R1. A number of definitions omit the "\lambda n", e.g. def 3.1 and 3.5, it would be better imo to include it.</t>
@@ -384,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -493,6 +496,30 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="11"/>
       </left>
       <right/>
@@ -528,7 +555,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -592,23 +619,53 @@
     <xf numFmtId="49" fontId="3" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="1"/>
@@ -1721,7 +1778,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1822,7 +1879,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s" s="12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
@@ -1830,10 +1887,10 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
@@ -1841,10 +1898,10 @@
     </row>
     <row r="11" ht="32.05" customHeight="1">
       <c r="A11" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s" s="7">
         <v>17</v>
-      </c>
-      <c r="B11" t="s" s="7">
-        <v>18</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
@@ -1852,10 +1909,10 @@
     </row>
     <row r="12" ht="68.05" customHeight="1">
       <c r="A12" t="s" s="16">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s" s="18">
         <v>19</v>
-      </c>
-      <c r="B12" t="s" s="18">
-        <v>20</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
@@ -1863,10 +1920,10 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s" s="12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
@@ -1874,10 +1931,10 @@
     </row>
     <row r="14" ht="32.05" customHeight="1">
       <c r="A14" t="s" s="19">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s" s="12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
@@ -1885,10 +1942,10 @@
     </row>
     <row r="15" ht="32.05" customHeight="1">
       <c r="A15" t="s" s="14">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
@@ -1896,10 +1953,10 @@
     </row>
     <row r="16" ht="32.05" customHeight="1">
       <c r="A16" t="s" s="19">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s" s="12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
@@ -1907,10 +1964,10 @@
     </row>
     <row r="17" ht="44.05" customHeight="1">
       <c r="A17" t="s" s="14">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
@@ -1918,10 +1975,10 @@
     </row>
     <row r="18" ht="56.05" customHeight="1">
       <c r="A18" t="s" s="14">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s" s="7">
         <v>26</v>
-      </c>
-      <c r="B18" t="s" s="7">
-        <v>27</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
@@ -1929,10 +1986,10 @@
     </row>
     <row r="19" ht="32.05" customHeight="1">
       <c r="A19" t="s" s="13">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s" s="12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
@@ -1940,10 +1997,10 @@
     </row>
     <row r="20" ht="44.05" customHeight="1">
       <c r="A20" t="s" s="19">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
@@ -1951,10 +2008,10 @@
     </row>
     <row r="21" ht="56.05" customHeight="1">
       <c r="A21" t="s" s="19">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
@@ -1962,10 +2019,10 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="19">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s" s="7">
         <v>31</v>
-      </c>
-      <c r="B22" t="s" s="7">
-        <v>32</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
@@ -1973,10 +2030,10 @@
     </row>
     <row r="23" ht="32.05" customHeight="1">
       <c r="A23" t="s" s="13">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s" s="12">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
@@ -1984,10 +2041,10 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="19">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
@@ -1995,7 +2052,7 @@
     </row>
     <row r="25" ht="48" customHeight="1">
       <c r="A25" t="s" s="19">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s" s="7">
         <v>11</v>
@@ -2006,10 +2063,10 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="19">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s" s="7">
         <v>36</v>
-      </c>
-      <c r="B26" t="s" s="7">
-        <v>37</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
@@ -2017,7 +2074,7 @@
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="19">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="8"/>
@@ -2026,10 +2083,10 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="20">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s" s="7">
         <v>39</v>
-      </c>
-      <c r="B28" t="s" s="7">
-        <v>40</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
@@ -2037,10 +2094,10 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="19">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
@@ -2048,197 +2105,195 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="19">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s" s="7">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
     </row>
     <row r="31" ht="32.05" customHeight="1">
-      <c r="A31" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="B31" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C31" s="8"/>
+      <c r="A31" t="s" s="21">
+        <v>42</v>
+      </c>
+      <c r="B31" s="22"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" ht="44.05" customHeight="1">
+    <row r="32" ht="32.05" customHeight="1">
       <c r="A32" t="s" s="19">
-        <v>45</v>
-      </c>
-      <c r="B32" t="s" s="7">
-        <v>46</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" ht="44.05" customHeight="1">
-      <c r="A33" t="s" s="20">
-        <v>47</v>
+    <row r="33" ht="32.05" customHeight="1">
+      <c r="A33" t="s" s="19">
+        <v>44</v>
       </c>
       <c r="B33" t="s" s="7">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="10"/>
     </row>
     <row r="34" ht="44.05" customHeight="1">
-      <c r="A34" t="s" s="20">
-        <v>49</v>
+      <c r="A34" t="s" s="19">
+        <v>46</v>
       </c>
       <c r="B34" t="s" s="7">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
     </row>
-    <row r="35" ht="32.05" customHeight="1">
-      <c r="A35" t="s" s="19">
-        <v>50</v>
+    <row r="35" ht="44.05" customHeight="1">
+      <c r="A35" t="s" s="20">
+        <v>48</v>
       </c>
       <c r="B35" t="s" s="7">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" ht="44.05" customHeight="1">
-      <c r="A36" t="s" s="19">
-        <v>52</v>
+      <c r="A36" t="s" s="20">
+        <v>50</v>
       </c>
       <c r="B36" t="s" s="7">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" ht="61.45" customHeight="1">
+    <row r="37" ht="32.05" customHeight="1">
       <c r="A37" t="s" s="19">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s" s="7">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
     </row>
-    <row r="38" ht="32.05" customHeight="1">
-      <c r="A38" t="s" s="20">
-        <v>55</v>
+    <row r="38" ht="44.05" customHeight="1">
+      <c r="A38" t="s" s="19">
+        <v>53</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
     </row>
-    <row r="39" ht="68.05" customHeight="1">
+    <row r="39" ht="61.45" customHeight="1">
       <c r="A39" t="s" s="19">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
     </row>
-    <row r="40" ht="56.05" customHeight="1">
+    <row r="40" ht="32.05" customHeight="1">
       <c r="A40" t="s" s="20">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s" s="7">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
     </row>
     <row r="41" ht="68.05" customHeight="1">
-      <c r="A41" t="s" s="20">
-        <v>61</v>
+      <c r="A41" t="s" s="19">
+        <v>58</v>
       </c>
       <c r="B41" t="s" s="7">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
     </row>
-    <row r="42" ht="32.05" customHeight="1">
-      <c r="A42" t="s" s="19">
-        <v>62</v>
+    <row r="42" ht="56.05" customHeight="1">
+      <c r="A42" t="s" s="20">
+        <v>60</v>
       </c>
       <c r="B42" t="s" s="7">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
     </row>
-    <row r="43" ht="32.05" customHeight="1">
-      <c r="A43" t="s" s="21">
-        <v>63</v>
-      </c>
-      <c r="B43" s="15"/>
+    <row r="43" ht="68.05" customHeight="1">
+      <c r="A43" t="s" s="20">
+        <v>62</v>
+      </c>
+      <c r="B43" t="s" s="7">
+        <v>57</v>
+      </c>
       <c r="C43" s="8"/>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" ht="32.05" customHeight="1">
-      <c r="A44" t="s" s="21">
-        <v>64</v>
-      </c>
-      <c r="B44" s="15"/>
+      <c r="A44" t="s" s="19">
+        <v>63</v>
+      </c>
+      <c r="B44" t="s" s="7">
+        <v>57</v>
+      </c>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
     </row>
     <row r="45" ht="32.05" customHeight="1">
-      <c r="A45" t="s" s="21">
-        <v>65</v>
+      <c r="A45" t="s" s="23">
+        <v>64</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" ht="92.05" customHeight="1">
-      <c r="A46" t="s" s="21">
-        <v>66</v>
+    <row r="46" ht="32.05" customHeight="1">
+      <c r="A46" t="s" s="23">
+        <v>65</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="10"/>
     </row>
-    <row r="47" ht="44.05" customHeight="1">
-      <c r="A47" t="s" s="20">
-        <v>67</v>
-      </c>
-      <c r="B47" t="s" s="7">
-        <v>68</v>
-      </c>
+    <row r="47" ht="32.05" customHeight="1">
+      <c r="A47" t="s" s="23">
+        <v>66</v>
+      </c>
+      <c r="B47" s="15"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="10"/>
     </row>
-    <row r="48" ht="32.05" customHeight="1">
-      <c r="A48" t="s" s="21">
-        <v>69</v>
+    <row r="48" ht="92.05" customHeight="1">
+      <c r="A48" t="s" s="23">
+        <v>67</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="8"/>
@@ -2246,17 +2301,19 @@
       <c r="E48" s="10"/>
     </row>
     <row r="49" ht="44.05" customHeight="1">
-      <c r="A49" t="s" s="21">
-        <v>70</v>
-      </c>
-      <c r="B49" s="15"/>
+      <c r="A49" t="s" s="20">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s" s="7">
+        <v>69</v>
+      </c>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" ht="44.05" customHeight="1">
-      <c r="A50" t="s" s="21">
-        <v>71</v>
+    <row r="50" ht="32.05" customHeight="1">
+      <c r="A50" t="s" s="23">
+        <v>70</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="8"/>
@@ -2264,21 +2321,39 @@
       <c r="E50" s="10"/>
     </row>
     <row r="51" ht="44.05" customHeight="1">
-      <c r="A51" t="s" s="21">
+      <c r="A51" t="s" s="23">
+        <v>71</v>
+      </c>
+      <c r="B51" s="15"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" ht="44.05" customHeight="1">
+      <c r="A52" t="s" s="23">
         <v>72</v>
       </c>
-      <c r="B51" s="15"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="24"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" ht="44.05" customHeight="1">
+      <c r="A53" t="s" s="23">
+        <v>73</v>
+      </c>
+      <c r="B53" s="15"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:B53"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:B42 A43:A51 B47">
+  <conditionalFormatting sqref="A2:B6 A7:A30 B8:B24 B26:B30 B32 A34:B44 A45:A53 B49">
     <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" text="Done.">
       <formula>FIND(UPPER("Done."),UPPER(A2))=1</formula>
       <formula>"Done."</formula>
@@ -2288,9 +2363,19 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B7 B25 A32:A33 B33">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" text="Done.">
+      <formula>FIND(UPPER("Done."),UPPER(B7))=1</formula>
+      <formula>"Done."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" text="Done">
+      <formula>FIND(UPPER("Done"),UPPER(B7))=1</formula>
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A49" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="A51" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="A51" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="A53" r:id="rId2" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Resolved issue 10 (listings all fit horizontally!). Created issue 33 for Linh.
</commit_message>
<xml_diff>
--- a/paper-aplas/known_issues_readable.xlsx
+++ b/paper-aplas/known_issues_readable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>Table 1</t>
   </si>
@@ -20,7 +20,7 @@
     <t xml:space="preserve">1. The historical note was a little off once we took out the binary stuff. Should have discussed multiplication, division, exponentiation, logs rather than numerical position systems. </t>
   </si>
   <si>
-    <t>Mostly okay, can expand if we have space.</t>
+    <t>Done, can expand if we have space.</t>
   </si>
   <si>
     <t>2. Need to sync up listings' line numbers with line numbers in code.</t>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>10. What shall we do about overflowing listings? There are quite a few in the new format, especially towards the end.</t>
-  </si>
-  <si>
-    <t>Do last</t>
   </si>
   <si>
     <t>11. &lt;&lt;We show that our functions run in $O(n)$ for inputs expressed in both unary and binary ($n$ = bitlength).&gt;&gt; Actually we didn't have any time complexity analysis for the inverse hyperoperations. The reader could figure out for themselves, but it's not explicitly stated in the paper. Aquinas: Ok, let's just add a sentance or two somewhere.</t>
@@ -192,13 +189,13 @@
     <t>30. Section 5.last, page 15 seems to have a typo?</t>
   </si>
   <si>
-    <t>Th 41. \forall i</t>
-  </si>
-  <si>
-    <t>Re-link to new repo</t>
-  </si>
-  <si>
-    <t>Anshuman changed some function names to make the listings fit, please reflect in codebase and in writing.</t>
+    <t>31. Th 41. \forall i</t>
+  </si>
+  <si>
+    <t>32. Make new anonymous repo and re-link theorems, definitions, proofs to new repo.</t>
+  </si>
+  <si>
+    <t>33. Anshuman changed some function names to make the listings fit, please reflect in codebase.</t>
   </si>
   <si>
     <t>R1. A number of definitions omit the "\lambda n", e.g. def 3.1 and 3.5, it would be better imo to include it.</t>
@@ -592,10 +589,10 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1814,7 +1811,7 @@
       <c r="A3" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="12">
+      <c r="B3" t="s" s="7">
         <v>4</v>
       </c>
       <c r="C3" s="8"/>
@@ -1822,10 +1819,10 @@
       <c r="E3" s="10"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="13">
+      <c r="A4" t="s" s="12">
         <v>5</v>
       </c>
-      <c r="B4" t="s" s="12">
+      <c r="B4" t="s" s="13">
         <v>6</v>
       </c>
       <c r="C4" s="8"/>
@@ -1864,7 +1861,7 @@
       <c r="E7" s="10"/>
     </row>
     <row r="8" ht="32.05" customHeight="1">
-      <c r="A8" t="s" s="13">
+      <c r="A8" t="s" s="12">
         <v>12</v>
       </c>
       <c r="B8" t="s" s="7">
@@ -1875,10 +1872,10 @@
       <c r="E8" s="10"/>
     </row>
     <row r="9" ht="32.05" customHeight="1">
-      <c r="A9" t="s" s="13">
+      <c r="A9" t="s" s="12">
         <v>14</v>
       </c>
-      <c r="B9" t="s" s="12">
+      <c r="B9" t="s" s="13">
         <v>11</v>
       </c>
       <c r="C9" s="8"/>
@@ -1901,7 +1898,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s" s="7">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
@@ -1909,20 +1906,20 @@
     </row>
     <row r="12" ht="68.05" customHeight="1">
       <c r="A12" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s" s="18">
         <v>18</v>
-      </c>
-      <c r="B12" t="s" s="18">
-        <v>19</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="13">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s" s="12">
+      <c r="A13" t="s" s="12">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s" s="13">
         <v>11</v>
       </c>
       <c r="C13" s="8"/>
@@ -1931,9 +1928,9 @@
     </row>
     <row r="14" ht="32.05" customHeight="1">
       <c r="A14" t="s" s="19">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s" s="13">
         <v>11</v>
       </c>
       <c r="C14" s="8"/>
@@ -1942,7 +1939,7 @@
     </row>
     <row r="15" ht="32.05" customHeight="1">
       <c r="A15" t="s" s="14">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s" s="7">
         <v>11</v>
@@ -1953,9 +1950,9 @@
     </row>
     <row r="16" ht="32.05" customHeight="1">
       <c r="A16" t="s" s="19">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s" s="13">
         <v>11</v>
       </c>
       <c r="C16" s="8"/>
@@ -1964,7 +1961,7 @@
     </row>
     <row r="17" ht="44.05" customHeight="1">
       <c r="A17" t="s" s="14">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s" s="7">
         <v>11</v>
@@ -1975,20 +1972,20 @@
     </row>
     <row r="18" ht="56.05" customHeight="1">
       <c r="A18" t="s" s="14">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s" s="7">
         <v>25</v>
-      </c>
-      <c r="B18" t="s" s="7">
-        <v>26</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
     </row>
     <row r="19" ht="32.05" customHeight="1">
-      <c r="A19" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s" s="12">
+      <c r="A19" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s" s="13">
         <v>11</v>
       </c>
       <c r="C19" s="8"/>
@@ -1997,7 +1994,7 @@
     </row>
     <row r="20" ht="44.05" customHeight="1">
       <c r="A20" t="s" s="19">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s" s="7">
         <v>11</v>
@@ -2008,7 +2005,7 @@
     </row>
     <row r="21" ht="56.05" customHeight="1">
       <c r="A21" t="s" s="19">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s" s="7">
         <v>11</v>
@@ -2019,20 +2016,20 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="19">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s" s="7">
         <v>30</v>
-      </c>
-      <c r="B22" t="s" s="7">
-        <v>31</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
     </row>
     <row r="23" ht="32.05" customHeight="1">
-      <c r="A23" t="s" s="13">
-        <v>32</v>
-      </c>
-      <c r="B23" t="s" s="12">
+      <c r="A23" t="s" s="12">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s" s="13">
         <v>11</v>
       </c>
       <c r="C23" s="8"/>
@@ -2041,7 +2038,7 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="19">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s" s="7">
         <v>11</v>
@@ -2052,7 +2049,7 @@
     </row>
     <row r="25" ht="48" customHeight="1">
       <c r="A25" t="s" s="19">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s" s="7">
         <v>11</v>
@@ -2063,10 +2060,10 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="19">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s" s="7">
         <v>35</v>
-      </c>
-      <c r="B26" t="s" s="7">
-        <v>36</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
@@ -2074,7 +2071,7 @@
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="19">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="8"/>
@@ -2083,10 +2080,10 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="20">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s" s="7">
         <v>38</v>
-      </c>
-      <c r="B28" t="s" s="7">
-        <v>39</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
@@ -2094,7 +2091,7 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="19">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s" s="7">
         <v>11</v>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="19">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s" s="7">
         <v>11</v>
@@ -2116,7 +2113,7 @@
     </row>
     <row r="31" ht="32.05" customHeight="1">
       <c r="A31" t="s" s="21">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B31" s="22"/>
       <c r="C31" s="9"/>
@@ -2125,19 +2122,21 @@
     </row>
     <row r="32" ht="32.05" customHeight="1">
       <c r="A32" t="s" s="19">
-        <v>43</v>
-      </c>
-      <c r="B32" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="B32" t="s" s="7">
+        <v>35</v>
+      </c>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
     </row>
     <row r="33" ht="32.05" customHeight="1">
       <c r="A33" t="s" s="19">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s" s="7">
         <v>44</v>
-      </c>
-      <c r="B33" t="s" s="7">
-        <v>45</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -2145,10 +2144,10 @@
     </row>
     <row r="34" ht="44.05" customHeight="1">
       <c r="A34" t="s" s="19">
+        <v>45</v>
+      </c>
+      <c r="B34" t="s" s="7">
         <v>46</v>
-      </c>
-      <c r="B34" t="s" s="7">
-        <v>47</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
@@ -2156,10 +2155,10 @@
     </row>
     <row r="35" ht="44.05" customHeight="1">
       <c r="A35" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s" s="7">
         <v>48</v>
-      </c>
-      <c r="B35" t="s" s="7">
-        <v>49</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
@@ -2167,7 +2166,7 @@
     </row>
     <row r="36" ht="44.05" customHeight="1">
       <c r="A36" t="s" s="20">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s" s="7">
         <v>11</v>
@@ -2178,10 +2177,10 @@
     </row>
     <row r="37" ht="32.05" customHeight="1">
       <c r="A37" t="s" s="19">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s" s="7">
         <v>51</v>
-      </c>
-      <c r="B37" t="s" s="7">
-        <v>52</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
@@ -2189,10 +2188,10 @@
     </row>
     <row r="38" ht="44.05" customHeight="1">
       <c r="A38" t="s" s="19">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s" s="7">
         <v>53</v>
-      </c>
-      <c r="B38" t="s" s="7">
-        <v>54</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
@@ -2200,7 +2199,7 @@
     </row>
     <row r="39" ht="61.45" customHeight="1">
       <c r="A39" t="s" s="19">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s" s="7">
         <v>11</v>
@@ -2211,10 +2210,10 @@
     </row>
     <row r="40" ht="32.05" customHeight="1">
       <c r="A40" t="s" s="20">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s" s="7">
         <v>56</v>
-      </c>
-      <c r="B40" t="s" s="7">
-        <v>57</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
@@ -2222,10 +2221,10 @@
     </row>
     <row r="41" ht="68.05" customHeight="1">
       <c r="A41" t="s" s="19">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s" s="7">
         <v>58</v>
-      </c>
-      <c r="B41" t="s" s="7">
-        <v>59</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
@@ -2233,10 +2232,10 @@
     </row>
     <row r="42" ht="56.05" customHeight="1">
       <c r="A42" t="s" s="20">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s" s="7">
         <v>60</v>
-      </c>
-      <c r="B42" t="s" s="7">
-        <v>61</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="9"/>
@@ -2244,10 +2243,10 @@
     </row>
     <row r="43" ht="68.05" customHeight="1">
       <c r="A43" t="s" s="20">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s" s="7">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="9"/>
@@ -2255,10 +2254,10 @@
     </row>
     <row r="44" ht="32.05" customHeight="1">
       <c r="A44" t="s" s="19">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s" s="7">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
@@ -2266,7 +2265,7 @@
     </row>
     <row r="45" ht="32.05" customHeight="1">
       <c r="A45" t="s" s="23">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="8"/>
@@ -2275,7 +2274,7 @@
     </row>
     <row r="46" ht="32.05" customHeight="1">
       <c r="A46" t="s" s="23">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="8"/>
@@ -2284,7 +2283,7 @@
     </row>
     <row r="47" ht="32.05" customHeight="1">
       <c r="A47" t="s" s="23">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="8"/>
@@ -2293,7 +2292,7 @@
     </row>
     <row r="48" ht="92.05" customHeight="1">
       <c r="A48" t="s" s="23">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="8"/>
@@ -2302,10 +2301,10 @@
     </row>
     <row r="49" ht="44.05" customHeight="1">
       <c r="A49" t="s" s="20">
+        <v>67</v>
+      </c>
+      <c r="B49" t="s" s="7">
         <v>68</v>
-      </c>
-      <c r="B49" t="s" s="7">
-        <v>69</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
@@ -2313,7 +2312,7 @@
     </row>
     <row r="50" ht="32.05" customHeight="1">
       <c r="A50" t="s" s="23">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="8"/>
@@ -2322,7 +2321,7 @@
     </row>
     <row r="51" ht="44.05" customHeight="1">
       <c r="A51" t="s" s="23">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="8"/>
@@ -2331,7 +2330,7 @@
     </row>
     <row r="52" ht="44.05" customHeight="1">
       <c r="A52" t="s" s="23">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B52" s="15"/>
       <c r="C52" s="8"/>
@@ -2340,7 +2339,7 @@
     </row>
     <row r="53" ht="44.05" customHeight="1">
       <c r="A53" t="s" s="23">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="24"/>
@@ -2353,7 +2352,7 @@
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="B49:B53"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:B6 A7:A30 B8:B24 B26:B30 B32 A34:B44 A45:A53 B49">
+  <conditionalFormatting sqref="A2:A12 B4:B6 B8:B10 B12 A13:B24 A25:A29 B26:B30 A34:B44 A45:A53 B49">
     <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" text="Done.">
       <formula>FIND(UPPER("Done."),UPPER(A2))=1</formula>
       <formula>"Done."</formula>
@@ -2363,13 +2362,13 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7 B25 A32:A33 B33">
+  <conditionalFormatting sqref="B2:B3 B7 B11 B25 A30 A32:B33">
     <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" text="Done.">
-      <formula>FIND(UPPER("Done."),UPPER(B7))=1</formula>
+      <formula>FIND(UPPER("Done."),UPPER(B2))=1</formula>
       <formula>"Done."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" text="Done">
-      <formula>FIND(UPPER("Done"),UPPER(B7))=1</formula>
+      <formula>FIND(UPPER("Done"),UPPER(B2))=1</formula>
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Polished some language, done with issue 4.
</commit_message>
<xml_diff>
--- a/paper-aplas/known_issues_readable.xlsx
+++ b/paper-aplas/known_issues_readable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
   <si>
     <t>Table 1</t>
   </si>
@@ -26,7 +26,7 @@
     <t>2. Need to sync up listings' line numbers with line numbers in code.</t>
   </si>
   <si>
-    <t>do last, when linking to Github</t>
+    <t>Unclear if needed.</t>
   </si>
   <si>
     <t xml:space="preserve">3. Notation of upper inverse is quite confusing with the -1 and the +. </t>
@@ -38,18 +38,18 @@
     <t>4. See Anshuman's inline notes throughout. They mark rough language that was a little too delicate for him to massage away.</t>
   </si>
   <si>
+    <t>Done.</t>
+  </si>
+  <si>
     <t>5. Test Makefile on different machines, slash remove it entirely and just give them a text-based order of compiling the files.</t>
   </si>
   <si>
-    <t>Do it properly, perhaps at the end.</t>
+    <t>Do at the end if we have time.</t>
   </si>
   <si>
     <t>6. Acknowledge Charguéraud and Pottier's repeater when introducing repeater</t>
   </si>
   <si>
-    <t>Done.</t>
-  </si>
-  <si>
     <t>7. Add a disclaimer that the practical hardcoded solution is obvious, we are trying to win in theory-land</t>
   </si>
   <si>
@@ -104,7 +104,7 @@
     <t>23. Add hyperlink to ack_hyperop in repeater.v when discussing kludge.</t>
   </si>
   <si>
-    <t>Later, when Github is stable.</t>
+    <t>Done, noted as part of a larger to-do.</t>
   </si>
   <si>
     <t>24. Use "inverse Ackermann" and "Inverse Ackermann" consistently. Right now captial I is used only in overview.tex</t>
@@ -174,28 +174,34 @@
     <t>27. Use Corollaries more.</t>
   </si>
   <si>
+    <t>Linh and Anshuman will do when linking on Monday.</t>
+  </si>
+  <si>
+    <t>28. Do we want a little \qed symbol after each proof?</t>
+  </si>
+  <si>
+    <t>Aquinas?</t>
+  </si>
+  <si>
+    <t>29. When do you mean O(n), \Theta(n), \Omega(n)?</t>
+  </si>
+  <si>
+    <t>Linh, change all \Theta to \bigO</t>
+  </si>
+  <si>
+    <t>30. Section 5.last, page 15 seems to have a typo?</t>
+  </si>
+  <si>
+    <t>31. Th 41. \forall i</t>
+  </si>
+  <si>
+    <t>32. Make new anonymous repo and re-link theorems, definitions, proofs to new repo.</t>
+  </si>
+  <si>
+    <t>33. Anshuman changed some function names to make the listings fit, please reflect in codebase.</t>
+  </si>
+  <si>
     <t>Linh.</t>
-  </si>
-  <si>
-    <t>28. Do we want a little \qed symbol after each proof?</t>
-  </si>
-  <si>
-    <t>29. When do you mean O(n), \Theta(n), \Omega(n)?</t>
-  </si>
-  <si>
-    <t>Linh, change all \Theta to \bigO</t>
-  </si>
-  <si>
-    <t>30. Section 5.last, page 15 seems to have a typo?</t>
-  </si>
-  <si>
-    <t>31. Th 41. \forall i</t>
-  </si>
-  <si>
-    <t>32. Make new anonymous repo and re-link theorems, definitions, proofs to new repo.</t>
-  </si>
-  <si>
-    <t>33. Anshuman changed some function names to make the listings fit, please reflect in codebase.</t>
   </si>
   <si>
     <t>R1. A number of definitions omit the "\lambda n", e.g. def 3.1 and 3.5, it would be better imo to include it.</t>
@@ -598,31 +604,31 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -638,31 +644,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="15"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color rgb="ff000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="14"/>
-          <bgColor indexed="15"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b val="1"/>
@@ -1833,28 +1815,30 @@
       <c r="A5" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" t="s" s="7">
+        <v>8</v>
+      </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" ht="32.05" customHeight="1">
-      <c r="A6" t="s" s="16">
-        <v>8</v>
+      <c r="A6" t="s" s="15">
+        <v>9</v>
       </c>
       <c r="B6" t="s" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" ht="32.05" customHeight="1">
-      <c r="A7" t="s" s="17">
-        <v>10</v>
+      <c r="A7" t="s" s="16">
+        <v>11</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
@@ -1876,7 +1860,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
@@ -1887,7 +1871,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
@@ -1898,17 +1882,17 @@
         <v>16</v>
       </c>
       <c r="B11" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
     </row>
     <row r="12" ht="68.05" customHeight="1">
-      <c r="A12" t="s" s="16">
+      <c r="A12" t="s" s="15">
         <v>17</v>
       </c>
-      <c r="B12" t="s" s="18">
+      <c r="B12" t="s" s="17">
         <v>18</v>
       </c>
       <c r="C12" s="8"/>
@@ -1920,18 +1904,18 @@
         <v>19</v>
       </c>
       <c r="B13" t="s" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
     </row>
     <row r="14" ht="32.05" customHeight="1">
-      <c r="A14" t="s" s="19">
+      <c r="A14" t="s" s="18">
         <v>20</v>
       </c>
       <c r="B14" t="s" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
@@ -1942,18 +1926,18 @@
         <v>21</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
     </row>
     <row r="16" ht="32.05" customHeight="1">
-      <c r="A16" t="s" s="19">
+      <c r="A16" t="s" s="18">
         <v>22</v>
       </c>
       <c r="B16" t="s" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
@@ -1964,7 +1948,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
@@ -1986,36 +1970,36 @@
         <v>26</v>
       </c>
       <c r="B19" t="s" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
     </row>
     <row r="20" ht="44.05" customHeight="1">
-      <c r="A20" t="s" s="19">
+      <c r="A20" t="s" s="18">
         <v>27</v>
       </c>
       <c r="B20" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
     </row>
     <row r="21" ht="56.05" customHeight="1">
-      <c r="A21" t="s" s="19">
+      <c r="A21" t="s" s="18">
         <v>28</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="10"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" t="s" s="19">
+      <c r="A22" t="s" s="18">
         <v>29</v>
       </c>
       <c r="B22" t="s" s="7">
@@ -2030,36 +2014,36 @@
         <v>31</v>
       </c>
       <c r="B23" t="s" s="13">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="19">
+      <c r="A24" t="s" s="18">
         <v>32</v>
       </c>
       <c r="B24" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
     </row>
     <row r="25" ht="48" customHeight="1">
-      <c r="A25" t="s" s="19">
+      <c r="A25" t="s" s="18">
         <v>33</v>
       </c>
       <c r="B25" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" t="s" s="19">
+      <c r="A26" t="s" s="18">
         <v>34</v>
       </c>
       <c r="B26" t="s" s="7">
@@ -2070,278 +2054,280 @@
       <c r="E26" s="10"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" t="s" s="19">
+      <c r="A27" t="s" s="18">
         <v>36</v>
       </c>
-      <c r="B27" s="15"/>
+      <c r="B27" t="s" s="7">
+        <v>37</v>
+      </c>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" t="s" s="20">
-        <v>37</v>
+      <c r="A28" t="s" s="19">
+        <v>38</v>
       </c>
       <c r="B28" t="s" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" t="s" s="19">
-        <v>39</v>
+      <c r="A29" t="s" s="18">
+        <v>40</v>
       </c>
       <c r="B29" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" t="s" s="19">
-        <v>40</v>
+      <c r="A30" t="s" s="18">
+        <v>41</v>
       </c>
       <c r="B30" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
     </row>
     <row r="31" ht="32.05" customHeight="1">
-      <c r="A31" t="s" s="21">
-        <v>41</v>
-      </c>
-      <c r="B31" s="22"/>
+      <c r="A31" t="s" s="20">
+        <v>42</v>
+      </c>
+      <c r="B31" s="21"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
     </row>
     <row r="32" ht="32.05" customHeight="1">
-      <c r="A32" t="s" s="19">
-        <v>42</v>
+      <c r="A32" t="s" s="18">
+        <v>43</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
     </row>
     <row r="33" ht="32.05" customHeight="1">
-      <c r="A33" t="s" s="19">
-        <v>43</v>
+      <c r="A33" t="s" s="18">
+        <v>45</v>
       </c>
       <c r="B33" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="10"/>
     </row>
     <row r="34" ht="44.05" customHeight="1">
-      <c r="A34" t="s" s="19">
-        <v>45</v>
+      <c r="A34" t="s" s="18">
+        <v>47</v>
       </c>
       <c r="B34" t="s" s="7">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
     </row>
     <row r="35" ht="44.05" customHeight="1">
-      <c r="A35" t="s" s="20">
-        <v>47</v>
+      <c r="A35" t="s" s="19">
+        <v>49</v>
       </c>
       <c r="B35" t="s" s="7">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" ht="44.05" customHeight="1">
-      <c r="A36" t="s" s="20">
-        <v>49</v>
+      <c r="A36" t="s" s="19">
+        <v>51</v>
       </c>
       <c r="B36" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
     </row>
     <row r="37" ht="32.05" customHeight="1">
-      <c r="A37" t="s" s="19">
-        <v>50</v>
+      <c r="A37" t="s" s="18">
+        <v>52</v>
       </c>
       <c r="B37" t="s" s="7">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
     </row>
     <row r="38" ht="44.05" customHeight="1">
-      <c r="A38" t="s" s="19">
-        <v>52</v>
+      <c r="A38" t="s" s="18">
+        <v>54</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
     </row>
     <row r="39" ht="61.45" customHeight="1">
-      <c r="A39" t="s" s="19">
-        <v>54</v>
+      <c r="A39" t="s" s="18">
+        <v>56</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
     </row>
     <row r="40" ht="32.05" customHeight="1">
-      <c r="A40" t="s" s="20">
-        <v>55</v>
+      <c r="A40" t="s" s="19">
+        <v>57</v>
       </c>
       <c r="B40" t="s" s="7">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
     </row>
     <row r="41" ht="68.05" customHeight="1">
-      <c r="A41" t="s" s="19">
-        <v>57</v>
+      <c r="A41" t="s" s="18">
+        <v>59</v>
       </c>
       <c r="B41" t="s" s="7">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
     </row>
     <row r="42" ht="56.05" customHeight="1">
-      <c r="A42" t="s" s="20">
-        <v>59</v>
+      <c r="A42" t="s" s="19">
+        <v>61</v>
       </c>
       <c r="B42" t="s" s="7">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" ht="68.05" customHeight="1">
-      <c r="A43" t="s" s="20">
-        <v>61</v>
+      <c r="A43" t="s" s="19">
+        <v>63</v>
       </c>
       <c r="B43" t="s" s="7">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" ht="32.05" customHeight="1">
-      <c r="A44" t="s" s="19">
-        <v>62</v>
+      <c r="A44" t="s" s="18">
+        <v>64</v>
       </c>
       <c r="B44" t="s" s="7">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
     </row>
     <row r="45" ht="32.05" customHeight="1">
-      <c r="A45" t="s" s="23">
-        <v>63</v>
-      </c>
-      <c r="B45" s="15"/>
+      <c r="A45" t="s" s="22">
+        <v>65</v>
+      </c>
+      <c r="B45" s="23"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
     </row>
     <row r="46" ht="32.05" customHeight="1">
-      <c r="A46" t="s" s="23">
-        <v>64</v>
-      </c>
-      <c r="B46" s="15"/>
+      <c r="A46" t="s" s="22">
+        <v>66</v>
+      </c>
+      <c r="B46" s="23"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="10"/>
     </row>
     <row r="47" ht="32.05" customHeight="1">
-      <c r="A47" t="s" s="23">
-        <v>65</v>
-      </c>
-      <c r="B47" s="15"/>
+      <c r="A47" t="s" s="22">
+        <v>67</v>
+      </c>
+      <c r="B47" s="23"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="10"/>
     </row>
     <row r="48" ht="92.05" customHeight="1">
-      <c r="A48" t="s" s="23">
-        <v>66</v>
-      </c>
-      <c r="B48" s="15"/>
+      <c r="A48" t="s" s="22">
+        <v>68</v>
+      </c>
+      <c r="B48" s="23"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="10"/>
     </row>
     <row r="49" ht="44.05" customHeight="1">
-      <c r="A49" t="s" s="20">
-        <v>67</v>
+      <c r="A49" t="s" s="19">
+        <v>69</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
     </row>
     <row r="50" ht="32.05" customHeight="1">
-      <c r="A50" t="s" s="23">
-        <v>69</v>
-      </c>
-      <c r="B50" s="15"/>
+      <c r="A50" t="s" s="22">
+        <v>71</v>
+      </c>
+      <c r="B50" s="23"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" ht="44.05" customHeight="1">
-      <c r="A51" t="s" s="23">
-        <v>70</v>
-      </c>
-      <c r="B51" s="15"/>
+      <c r="A51" t="s" s="22">
+        <v>72</v>
+      </c>
+      <c r="B51" s="23"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" ht="44.05" customHeight="1">
-      <c r="A52" t="s" s="23">
-        <v>71</v>
-      </c>
-      <c r="B52" s="15"/>
+      <c r="A52" t="s" s="22">
+        <v>73</v>
+      </c>
+      <c r="B52" s="23"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="10"/>
     </row>
     <row r="53" ht="44.05" customHeight="1">
-      <c r="A53" t="s" s="23">
-        <v>72</v>
-      </c>
-      <c r="B53" s="15"/>
+      <c r="A53" t="s" s="22">
+        <v>74</v>
+      </c>
+      <c r="B53" s="23"/>
       <c r="C53" s="24"/>
       <c r="D53" s="25"/>
       <c r="E53" s="26"/>
@@ -2352,23 +2338,13 @@
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="B49:B53"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:A12 B4:B6 B8:B10 B12 A13:B24 A25:A29 B26:B30 A34:B44 A45:A53 B49">
+  <conditionalFormatting sqref="A2:B30 A32:B44 A45:A53 B49">
     <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" text="Done.">
       <formula>FIND(UPPER("Done."),UPPER(A2))=1</formula>
       <formula>"Done."</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" text="Done">
       <formula>FIND(UPPER("Done"),UPPER(A2))=1</formula>
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B7 B11 B25 A30 A32:B33">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" text="Done.">
-      <formula>FIND(UPPER("Done."),UPPER(B2))=1</formula>
-      <formula>"Done."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" text="Done">
-      <formula>FIND(UPPER("Done"),UPPER(B2))=1</formula>
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Cleaned up repo by deleting many unused files.
</commit_message>
<xml_diff>
--- a/paper-aplas/known_issues_readable.xlsx
+++ b/paper-aplas/known_issues_readable.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>Table 1</t>
   </si>
@@ -26,7 +26,7 @@
     <t>2. Need to sync up listings' line numbers with line numbers in code.</t>
   </si>
   <si>
-    <t>Unclear if needed.</t>
+    <t>Done.</t>
   </si>
   <si>
     <t xml:space="preserve">3. Notation of upper inverse is quite confusing with the -1 and the +. </t>
@@ -38,15 +38,9 @@
     <t>4. See Anshuman's inline notes throughout. They mark rough language that was a little too delicate for him to massage away.</t>
   </si>
   <si>
-    <t>Done.</t>
-  </si>
-  <si>
     <t>5. Test Makefile on different machines, slash remove it entirely and just give them a text-based order of compiling the files.</t>
   </si>
   <si>
-    <t>Do at the end if we have time.</t>
-  </si>
-  <si>
     <t>6. Acknowledge Charguéraud and Pottier's repeater when introducing repeater</t>
   </si>
   <si>
@@ -68,7 +62,7 @@
     <t>11. &lt;&lt;We show that our functions run in $O(n)$ for inputs expressed in both unary and binary ($n$ = bitlength).&gt;&gt; Actually we didn't have any time complexity analysis for the inverse hyperoperations. The reader could figure out for themselves, but it's not explicitly stated in the paper. Aquinas: Ok, let's just add a sentance or two somewhere.</t>
   </si>
   <si>
-    <t>Linh, double-check hyperops in bin.</t>
+    <t>Done, Aquinas is taking care of it.</t>
   </si>
   <si>
     <t>12. I want to massage away the bold in Section 3.2.</t>
@@ -174,21 +168,15 @@
     <t>27. Use Corollaries more.</t>
   </si>
   <si>
-    <t>Linh and Anshuman will do when linking on Monday.</t>
-  </si>
-  <si>
     <t>28. Do we want a little \qed symbol after each proof?</t>
   </si>
   <si>
-    <t>Aquinas?</t>
+    <t>Done, not doing.</t>
   </si>
   <si>
     <t>29. When do you mean O(n), \Theta(n), \Omega(n)?</t>
   </si>
   <si>
-    <t>Linh, change all \Theta to \bigO</t>
-  </si>
-  <si>
     <t>30. Section 5.last, page 15 seems to have a typo?</t>
   </si>
   <si>
@@ -201,21 +189,12 @@
     <t>33. Anshuman changed some function names to make the listings fit, please reflect in codebase.</t>
   </si>
   <si>
-    <t>Linh.</t>
-  </si>
-  <si>
     <t>R1. A number of definitions omit the "\lambda n", e.g. def 3.1 and 3.5, it would be better imo to include it.</t>
   </si>
   <si>
-    <t>Consider carefully at the end.</t>
-  </si>
-  <si>
     <t>R2. The key idea is about hyperoperations, a beautiful generalization of what the Ackermann function is trying to do, and IMO the "right way" to do it. Why don't you start with hyperoperations in the introduction?</t>
   </si>
   <si>
-    <t>Aquinas will look at the intro</t>
-  </si>
-  <si>
     <t>R3. Section 2: "Let us now consider hyperoperations more carefully" - we haven't really considered them so far, only seen some examples, so this was really confusing to me.</t>
   </si>
   <si>
@@ -226,9 +205,6 @@
   </si>
   <si>
     <t>R5: Don't cramp the three cases of the formal defn of hyperoperations into one line. It is too important.</t>
-  </si>
-  <si>
-    <t>Consider last, in case there is space.</t>
   </si>
   <si>
     <t>R6. Section 3.1, about inverses, I would like to see some kind of graph, to understand what is going on. Or/and perhaps an example of an inverse to start with before seeing the definition (to complement lines 183 and 184).</t>
@@ -309,6 +285,52 @@
       <t>https://github.com/math-comp/math-comp/blob/9d8e99f50e1f00413c355277123a70e497491afc/mathcomp/ssreflect/prime.v#L48</t>
     </r>
   </si>
+  <si>
+    <t>defn: inv-ack-new</t>
+  </si>
+  <si>
+    <t>Clean up the comment headings of the code files. Maybe add numbers to them for indexing.</t>
+  </si>
+  <si>
+    <t>Comment in bin_inverse.v for Linh.</t>
+  </si>
+  <si>
+    <t>.bbl and add a \vpsace{-0.25em}</t>
+  </si>
+  <si>
+    <t>Done, no longer needed.</t>
+  </si>
+  <si>
+    <t>Can edit theorem 14 to remove &gt;= a+1?</t>
+  </si>
+  <si>
+    <t>Use mathfont consistently for log and log*. Ref table vs section 4, for an example.</t>
+  </si>
+  <si>
+    <t>Done, maybe ask Aquinas if he wants to revert.</t>
+  </si>
+  <si>
+    <t>Can lose the “when alpha is defined per 24”. It is a redefinition, the latter applies.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Listings google sheet: </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://docs.google.com/spreadsheets/d/1H9R3L1Qtr6jju7QkOjLIiejX-P8CK6QowB5WHlMALYE/edit?usp=sharing</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -317,7 +339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -343,6 +365,12 @@
       <u val="single"/>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="20"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -390,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -501,18 +529,9 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
@@ -552,13 +571,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -622,29 +678,62 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color rgb="ff000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="14"/>
+          <bgColor indexed="15"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="1"/>
@@ -693,6 +782,7 @@
       <rgbColor rgb="fff8ba00"/>
       <rgbColor rgb="fffefefe"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1757,7 +1847,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1816,7 +1906,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="9"/>
@@ -1824,10 +1914,10 @@
     </row>
     <row r="6" ht="32.05" customHeight="1">
       <c r="A6" t="s" s="15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s" s="7">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
@@ -1835,10 +1925,10 @@
     </row>
     <row r="7" ht="32.05" customHeight="1">
       <c r="A7" t="s" s="16">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
@@ -1846,10 +1936,10 @@
     </row>
     <row r="8" ht="32.05" customHeight="1">
       <c r="A8" t="s" s="12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s" s="7">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="9"/>
@@ -1857,10 +1947,10 @@
     </row>
     <row r="9" ht="32.05" customHeight="1">
       <c r="A9" t="s" s="12">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
@@ -1868,10 +1958,10 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="14">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
@@ -1879,10 +1969,10 @@
     </row>
     <row r="11" ht="32.05" customHeight="1">
       <c r="A11" t="s" s="11">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
@@ -1890,10 +1980,10 @@
     </row>
     <row r="12" ht="68.05" customHeight="1">
       <c r="A12" t="s" s="15">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s" s="17">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
@@ -1901,10 +1991,10 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="12">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
@@ -1912,10 +2002,10 @@
     </row>
     <row r="14" ht="32.05" customHeight="1">
       <c r="A14" t="s" s="18">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
@@ -1923,10 +2013,10 @@
     </row>
     <row r="15" ht="32.05" customHeight="1">
       <c r="A15" t="s" s="14">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="9"/>
@@ -1934,10 +2024,10 @@
     </row>
     <row r="16" ht="32.05" customHeight="1">
       <c r="A16" t="s" s="18">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
@@ -1945,10 +2035,10 @@
     </row>
     <row r="17" ht="44.05" customHeight="1">
       <c r="A17" t="s" s="14">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
@@ -1956,10 +2046,10 @@
     </row>
     <row r="18" ht="56.05" customHeight="1">
       <c r="A18" t="s" s="14">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s" s="7">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
@@ -1967,10 +2057,10 @@
     </row>
     <row r="19" ht="32.05" customHeight="1">
       <c r="A19" t="s" s="12">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
@@ -1978,10 +2068,10 @@
     </row>
     <row r="20" ht="44.05" customHeight="1">
       <c r="A20" t="s" s="18">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
@@ -1989,10 +2079,10 @@
     </row>
     <row r="21" ht="56.05" customHeight="1">
       <c r="A21" t="s" s="18">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
@@ -2000,10 +2090,10 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="18">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s" s="7">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
@@ -2011,10 +2101,10 @@
     </row>
     <row r="23" ht="32.05" customHeight="1">
       <c r="A23" t="s" s="12">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s" s="13">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
@@ -2022,10 +2112,10 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="18">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="9"/>
@@ -2033,10 +2123,10 @@
     </row>
     <row r="25" ht="48" customHeight="1">
       <c r="A25" t="s" s="18">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="9"/>
@@ -2044,10 +2134,10 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="18">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s" s="7">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="9"/>
@@ -2055,10 +2145,10 @@
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="18">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s" s="7">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
@@ -2066,10 +2156,10 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="19">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s" s="7">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
@@ -2077,10 +2167,10 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="18">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
@@ -2088,10 +2178,10 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="18">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="9"/>
@@ -2099,19 +2189,21 @@
     </row>
     <row r="31" ht="32.05" customHeight="1">
       <c r="A31" t="s" s="20">
-        <v>42</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="B31" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C31" s="8"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
     </row>
     <row r="32" ht="32.05" customHeight="1">
       <c r="A32" t="s" s="18">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
@@ -2119,10 +2211,10 @@
     </row>
     <row r="33" ht="32.05" customHeight="1">
       <c r="A33" t="s" s="18">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s" s="7">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
@@ -2130,10 +2222,10 @@
     </row>
     <row r="34" ht="44.05" customHeight="1">
       <c r="A34" t="s" s="18">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s" s="7">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
@@ -2141,10 +2233,10 @@
     </row>
     <row r="35" ht="44.05" customHeight="1">
       <c r="A35" t="s" s="19">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B35" t="s" s="7">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
@@ -2152,10 +2244,10 @@
     </row>
     <row r="36" ht="44.05" customHeight="1">
       <c r="A36" t="s" s="19">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
@@ -2163,10 +2255,10 @@
     </row>
     <row r="37" ht="32.05" customHeight="1">
       <c r="A37" t="s" s="18">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B37" t="s" s="7">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
@@ -2174,10 +2266,10 @@
     </row>
     <row r="38" ht="44.05" customHeight="1">
       <c r="A38" t="s" s="18">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s" s="7">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
@@ -2185,10 +2277,10 @@
     </row>
     <row r="39" ht="61.45" customHeight="1">
       <c r="A39" t="s" s="18">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
@@ -2196,10 +2288,10 @@
     </row>
     <row r="40" ht="32.05" customHeight="1">
       <c r="A40" t="s" s="19">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s" s="7">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
@@ -2207,10 +2299,10 @@
     </row>
     <row r="41" ht="68.05" customHeight="1">
       <c r="A41" t="s" s="18">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s" s="7">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
@@ -2218,10 +2310,10 @@
     </row>
     <row r="42" ht="56.05" customHeight="1">
       <c r="A42" t="s" s="19">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s" s="7">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="9"/>
@@ -2229,10 +2321,10 @@
     </row>
     <row r="43" ht="68.05" customHeight="1">
       <c r="A43" t="s" s="19">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B43" t="s" s="7">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="9"/>
@@ -2240,97 +2332,185 @@
     </row>
     <row r="44" ht="32.05" customHeight="1">
       <c r="A44" t="s" s="18">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B44" t="s" s="7">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
     </row>
     <row r="45" ht="32.05" customHeight="1">
-      <c r="A45" t="s" s="22">
-        <v>65</v>
-      </c>
-      <c r="B45" s="23"/>
+      <c r="A45" t="s" s="21">
+        <v>57</v>
+      </c>
+      <c r="B45" s="22"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
     </row>
     <row r="46" ht="32.05" customHeight="1">
-      <c r="A46" t="s" s="22">
-        <v>66</v>
-      </c>
-      <c r="B46" s="23"/>
+      <c r="A46" t="s" s="21">
+        <v>58</v>
+      </c>
+      <c r="B46" s="22"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="10"/>
     </row>
     <row r="47" ht="32.05" customHeight="1">
-      <c r="A47" t="s" s="22">
-        <v>67</v>
-      </c>
-      <c r="B47" s="23"/>
+      <c r="A47" t="s" s="21">
+        <v>59</v>
+      </c>
+      <c r="B47" s="22"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="10"/>
     </row>
     <row r="48" ht="92.05" customHeight="1">
-      <c r="A48" t="s" s="22">
-        <v>68</v>
-      </c>
-      <c r="B48" s="23"/>
+      <c r="A48" t="s" s="21">
+        <v>60</v>
+      </c>
+      <c r="B48" s="22"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="10"/>
     </row>
     <row r="49" ht="44.05" customHeight="1">
       <c r="A49" t="s" s="19">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
     </row>
     <row r="50" ht="32.05" customHeight="1">
-      <c r="A50" t="s" s="22">
-        <v>71</v>
-      </c>
-      <c r="B50" s="23"/>
+      <c r="A50" t="s" s="21">
+        <v>63</v>
+      </c>
+      <c r="B50" s="22"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" ht="44.05" customHeight="1">
-      <c r="A51" t="s" s="22">
-        <v>72</v>
-      </c>
-      <c r="B51" s="23"/>
+      <c r="A51" t="s" s="21">
+        <v>64</v>
+      </c>
+      <c r="B51" s="22"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" ht="44.05" customHeight="1">
-      <c r="A52" t="s" s="22">
-        <v>73</v>
-      </c>
-      <c r="B52" s="23"/>
+      <c r="A52" t="s" s="21">
+        <v>65</v>
+      </c>
+      <c r="B52" s="22"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="10"/>
     </row>
     <row r="53" ht="44.05" customHeight="1">
-      <c r="A53" t="s" s="22">
+      <c r="A53" t="s" s="21">
+        <v>66</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="25"/>
+    </row>
+    <row r="54" ht="44.05" customHeight="1">
+      <c r="A54" t="s" s="26">
+        <v>67</v>
+      </c>
+      <c r="B54" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C54" s="27"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="29"/>
+    </row>
+    <row r="55" ht="44.05" customHeight="1">
+      <c r="A55" t="s" s="26">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="29"/>
+    </row>
+    <row r="56" ht="44.05" customHeight="1">
+      <c r="A56" t="s" s="26">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C56" s="27"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="29"/>
+    </row>
+    <row r="57" ht="44.05" customHeight="1">
+      <c r="A57" t="s" s="26">
+        <v>70</v>
+      </c>
+      <c r="B57" t="s" s="7">
+        <v>71</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="29"/>
+    </row>
+    <row r="58" ht="44.05" customHeight="1">
+      <c r="A58" t="s" s="26">
+        <v>72</v>
+      </c>
+      <c r="B58" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C58" s="27"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="29"/>
+    </row>
+    <row r="59" ht="44.05" customHeight="1">
+      <c r="A59" t="s" s="26">
+        <v>73</v>
+      </c>
+      <c r="B59" t="s" s="7">
         <v>74</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="26"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="29"/>
+    </row>
+    <row r="60" ht="44.05" customHeight="1">
+      <c r="A60" t="s" s="26">
+        <v>75</v>
+      </c>
+      <c r="B60" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C60" s="27"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="29"/>
+    </row>
+    <row r="61" ht="44.05" customHeight="1">
+      <c r="A61" t="s" s="26">
+        <v>76</v>
+      </c>
+      <c r="B61" t="s" s="7">
+        <v>4</v>
+      </c>
+      <c r="C61" s="27"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2338,7 +2518,7 @@
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="B49:B53"/>
   </mergeCells>
-  <conditionalFormatting sqref="A2:B30 A32:B44 A45:A53 B49">
+  <conditionalFormatting sqref="A2:B30 A32:B44 A45:A60 B49 B54:B60">
     <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" text="Done.">
       <formula>FIND(UPPER("Done."),UPPER(A2))=1</formula>
       <formula>"Done."</formula>
@@ -2348,9 +2528,20 @@
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B31 A61:B61">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" text="Done.">
+      <formula>FIND(UPPER("Done."),UPPER(B31))=1</formula>
+      <formula>"Done."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" text="Done">
+      <formula>FIND(UPPER("Done"),UPPER(B31))=1</formula>
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A51" r:id="rId1" location="" tooltip="" display=""/>
     <hyperlink ref="A53" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="A61" r:id="rId3" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>